<commit_message>
Wargame data and updates to equipment database
</commit_message>
<xml_diff>
--- a/_reference/Berlin OOBs.xlsx
+++ b/_reference/Berlin OOBs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Berlin Bde" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="1st MRD (DDR)" sheetId="21" r:id="rId6"/>
     <sheet name="DDR Border Rgts" sheetId="23" r:id="rId7"/>
     <sheet name="DDR other" sheetId="22" r:id="rId8"/>
+    <sheet name="BRD Fallschirmjaeger" sheetId="25" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="173">
   <si>
     <t>TOTAL</t>
   </si>
@@ -513,6 +514,51 @@
   <si>
     <t>West Berlin Police
 36 companies</t>
+  </si>
+  <si>
+    <t>HQ company</t>
+  </si>
+  <si>
+    <t>Fallschirmjaeger btn</t>
+  </si>
+  <si>
+    <t>AT btn</t>
+  </si>
+  <si>
+    <t>Supply co</t>
+  </si>
+  <si>
+    <t>Transport co</t>
+  </si>
+  <si>
+    <t>Medical co</t>
+  </si>
+  <si>
+    <t>Engineer co</t>
+  </si>
+  <si>
+    <t>TOW</t>
+  </si>
+  <si>
+    <t>Rh202</t>
+  </si>
+  <si>
+    <t>Kraka</t>
+  </si>
+  <si>
+    <t>Iltis</t>
+  </si>
+  <si>
+    <t>Fallschirmjaeger co</t>
+  </si>
+  <si>
+    <t>Heavy company</t>
+  </si>
+  <si>
+    <t>PzF-44-1</t>
+  </si>
+  <si>
+    <t>MG3</t>
   </si>
 </sst>
 </file>
@@ -996,27 +1042,27 @@
         <v>3668</v>
       </c>
       <c r="D2" s="3">
-        <f>SUMPRODUCT(D3:D30,$B$3:$B$30)</f>
+        <f t="shared" ref="D2:I2" si="1">SUMPRODUCT(D3:D30,$B$3:$B$30)</f>
         <v>554</v>
       </c>
       <c r="E2" s="3">
-        <f>SUMPRODUCT(E3:E30,$B$3:$B$30)</f>
+        <f t="shared" si="1"/>
         <v>554</v>
       </c>
       <c r="F2" s="3">
-        <f>SUMPRODUCT(F3:F30,$B$3:$B$30)</f>
+        <f t="shared" si="1"/>
         <v>554</v>
       </c>
       <c r="G2" s="3">
-        <f>SUMPRODUCT(G3:G30,$B$3:$B$30)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="H2" s="3">
-        <f>SUMPRODUCT(H3:H30,$B$3:$B$30)</f>
+        <f t="shared" si="1"/>
         <v>1860</v>
       </c>
       <c r="I2" s="3">
-        <f>SUMPRODUCT(I3:I30,$B$3:$B$30)</f>
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
       <c r="J2" s="3"/>
@@ -1102,11 +1148,11 @@
         <v>303</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" ref="E5:F5" si="1">3*(11+3*30)</f>
+        <f t="shared" ref="E5:F5" si="2">3*(11+3*30)</f>
         <v>303</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>303</v>
       </c>
       <c r="G5" s="3">
@@ -1143,11 +1189,11 @@
         <v>33</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" ref="E6:F6" si="2">3*3*3+6</f>
+        <f t="shared" ref="E6:F6" si="3">3*3*3+6</f>
         <v>33</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="G6" s="3"/>
@@ -1180,11 +1226,11 @@
         <v>54</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" ref="E7:F7" si="3">3*3*3*2</f>
+        <f t="shared" ref="E7:F7" si="4">3*3*3*2</f>
         <v>54</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="G7" s="3"/>
@@ -1355,7 +1401,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="9">
-        <f t="shared" ref="C13" si="4">SUM(D13:P13)</f>
+        <f t="shared" ref="C13" si="5">SUM(D13:P13)</f>
         <v>36</v>
       </c>
       <c r="D13" s="3">
@@ -1383,7 +1429,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="9">
-        <f t="shared" ref="C14" si="5">SUM(D14:P14)</f>
+        <f t="shared" ref="C14" si="6">SUM(D14:P14)</f>
         <v>50</v>
       </c>
       <c r="D14" s="3"/>
@@ -2424,7 +2470,7 @@
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="9">
-        <f>SUM(D2:O2)</f>
+        <f t="shared" ref="C2:C15" si="0">SUM(D2:O2)</f>
         <v>1326</v>
       </c>
       <c r="D2" s="3">
@@ -2432,15 +2478,15 @@
         <v>938</v>
       </c>
       <c r="E2" s="3">
-        <f t="shared" ref="E2:I2" si="0">SUMPRODUCT(E3:E33,$B$3:$B$33)</f>
+        <f t="shared" ref="E2:G2" si="1">SUMPRODUCT(E3:E33,$B$3:$B$33)</f>
         <v>388</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G2" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H2" s="3"/>
@@ -2455,7 +2501,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="9">
-        <f>SUM(D3:O3)</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="D3" s="3"/>
@@ -2475,7 +2521,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="9">
-        <f>SUM(D4:O4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D4" s="3"/>
@@ -2495,7 +2541,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="9">
-        <f>SUM(D5:O5)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="D5" s="3"/>
@@ -2515,7 +2561,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="9">
-        <f>SUM(D6:O6)</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="D6" s="3">
@@ -2534,7 +2580,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="9">
-        <f>SUM(D7:O7)</f>
+        <f t="shared" si="0"/>
         <v>517</v>
       </c>
       <c r="D7" s="3">
@@ -2557,7 +2603,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="9">
-        <f>SUM(D8:O8)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="D8" s="3">
@@ -2580,7 +2626,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="9">
-        <f>SUM(D9:O9)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="D9" s="3">
@@ -2603,7 +2649,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="9">
-        <f>SUM(D10:O10)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="D10" s="3">
@@ -2622,7 +2668,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="9">
-        <f>SUM(D11:O11)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="D11" s="3">
@@ -2641,7 +2687,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="9">
-        <f>SUM(D12:O12)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D12" s="3">
@@ -2660,7 +2706,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="9">
-        <f>SUM(D13:O13)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D13" s="3">
@@ -2679,7 +2725,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="9">
-        <f>SUM(D14:O14)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D14" s="3">
@@ -2698,7 +2744,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="9">
-        <f>SUM(D15:O15)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D15" s="3">
@@ -2777,31 +2823,31 @@
         <v>2488</v>
       </c>
       <c r="D2" s="3">
-        <f>SUMPRODUCT(D3:D29,$B$3:$B$29)</f>
+        <f t="shared" ref="D2:J2" si="1">SUMPRODUCT(D3:D29,$B$3:$B$29)</f>
         <v>472</v>
       </c>
       <c r="E2" s="3">
-        <f>SUMPRODUCT(E3:E29,$B$3:$B$29)</f>
+        <f t="shared" si="1"/>
         <v>472</v>
       </c>
       <c r="F2" s="3">
-        <f>SUMPRODUCT(F3:F29,$B$3:$B$29)</f>
+        <f t="shared" si="1"/>
         <v>472</v>
       </c>
       <c r="G2" s="3">
-        <f>SUMPRODUCT(G3:G29,$B$3:$B$29)</f>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="H2" s="3">
-        <f>SUMPRODUCT(H3:H29,$B$3:$B$29)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I2" s="3">
-        <f>SUMPRODUCT(I3:I29,$B$3:$B$29)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J2" s="3">
-        <f>SUMPRODUCT(J3:J29,$B$3:$B$29)</f>
+        <f t="shared" si="1"/>
         <v>996</v>
       </c>
     </row>
@@ -3166,27 +3212,27 @@
         <v>10476</v>
       </c>
       <c r="D2" s="3">
-        <f>SUMPRODUCT(D3:D29,$B$3:$B$29)</f>
+        <f t="shared" ref="D2:I2" si="1">SUMPRODUCT(D3:D29,$B$3:$B$29)</f>
         <v>1746</v>
       </c>
       <c r="E2" s="3">
-        <f>SUMPRODUCT(E3:E29,$B$3:$B$29)</f>
+        <f t="shared" si="1"/>
         <v>1746</v>
       </c>
       <c r="F2" s="3">
-        <f>SUMPRODUCT(F3:F29,$B$3:$B$29)</f>
+        <f t="shared" si="1"/>
         <v>1746</v>
       </c>
       <c r="G2" s="3">
-        <f>SUMPRODUCT(G3:G29,$B$3:$B$29)</f>
+        <f t="shared" si="1"/>
         <v>1746</v>
       </c>
       <c r="H2" s="3">
-        <f>SUMPRODUCT(H3:H29,$B$3:$B$29)</f>
+        <f t="shared" si="1"/>
         <v>1746</v>
       </c>
       <c r="I2" s="3">
-        <f>SUMPRODUCT(I3:I29,$B$3:$B$29)</f>
+        <f t="shared" si="1"/>
         <v>1746</v>
       </c>
     </row>
@@ -5673,8 +5719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6318,4 +6364,794 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" customWidth="1"/>
+    <col min="23" max="23" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.85546875" customWidth="1"/>
+    <col min="25" max="25" width="6.28515625" customWidth="1"/>
+    <col min="26" max="26" width="7" customWidth="1"/>
+    <col min="27" max="27" width="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="T1" s="2"/>
+      <c r="U1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="X1" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y1" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z1" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="AA1" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="9">
+        <f>SUM(D2:O2)</f>
+        <v>2332</v>
+      </c>
+      <c r="D2" s="3">
+        <f>SUMPRODUCT(D3:D54,$B$3:$B$54)</f>
+        <v>42</v>
+      </c>
+      <c r="E2" s="3">
+        <f>SUMPRODUCT(E3:E54,$B$3:$B$54)</f>
+        <v>576</v>
+      </c>
+      <c r="F2" s="3">
+        <f>SUMPRODUCT(F3:F54,$B$3:$B$54)</f>
+        <v>576</v>
+      </c>
+      <c r="G2" s="3">
+        <f>SUMPRODUCT(G3:G54,$B$3:$B$54)</f>
+        <v>384</v>
+      </c>
+      <c r="H2" s="3">
+        <f>SUMPRODUCT(H3:H54,$B$3:$B$54)</f>
+        <v>384</v>
+      </c>
+      <c r="I2" s="3">
+        <f>SUMPRODUCT(I3:I54,$B$3:$B$54)</f>
+        <v>90</v>
+      </c>
+      <c r="J2" s="3">
+        <f>SUMPRODUCT(J3:J54,$B$3:$B$54)</f>
+        <v>78</v>
+      </c>
+      <c r="K2" s="3">
+        <f>SUMPRODUCT(K3:K54,$B$3:$B$54)</f>
+        <v>48</v>
+      </c>
+      <c r="L2" s="3">
+        <f>SUMPRODUCT(L3:L54,$B$3:$B$54)</f>
+        <v>154</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="12"/>
+      <c r="V2" s="9">
+        <f>SUM(W2:AA2)</f>
+        <v>576</v>
+      </c>
+      <c r="W2" s="3">
+        <f>SUMPRODUCT(W3:W16,$U$3:$U$16)</f>
+        <v>72</v>
+      </c>
+      <c r="X2" s="3">
+        <f t="shared" ref="X2:AA2" si="0">SUMPRODUCT(X3:X16,$U$3:$U$16)</f>
+        <v>120</v>
+      </c>
+      <c r="Y2" s="3">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="Z2" s="3">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="AA2" s="3">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <f t="shared" ref="C3:C16" si="1">SUM(D3:O3)</f>
+        <v>1316</v>
+      </c>
+      <c r="D3" s="3">
+        <v>20</v>
+      </c>
+      <c r="E3" s="21">
+        <v>366</v>
+      </c>
+      <c r="F3" s="21">
+        <v>366</v>
+      </c>
+      <c r="G3" s="3">
+        <f>6*G4</f>
+        <v>180</v>
+      </c>
+      <c r="H3" s="3">
+        <f>6*H4</f>
+        <v>180</v>
+      </c>
+      <c r="I3" s="3">
+        <v>40</v>
+      </c>
+      <c r="J3" s="3">
+        <v>18</v>
+      </c>
+      <c r="K3" s="3">
+        <v>48</v>
+      </c>
+      <c r="L3" s="3">
+        <v>98</v>
+      </c>
+      <c r="T3" t="s">
+        <v>147</v>
+      </c>
+      <c r="U3" s="12">
+        <v>1</v>
+      </c>
+      <c r="V3" s="9">
+        <f t="shared" ref="V3:V16" si="2">SUM(W3:AA3)</f>
+        <v>366</v>
+      </c>
+      <c r="W3" s="3">
+        <v>60</v>
+      </c>
+      <c r="X3" s="3">
+        <v>82</v>
+      </c>
+      <c r="Y3" s="21">
+        <f>X3</f>
+        <v>82</v>
+      </c>
+      <c r="Z3" s="3">
+        <f>X3</f>
+        <v>82</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="12">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="21">
+        <v>10</v>
+      </c>
+      <c r="F4" s="21">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3">
+        <v>30</v>
+      </c>
+      <c r="H4" s="3">
+        <v>30</v>
+      </c>
+      <c r="T4" t="s">
+        <v>165</v>
+      </c>
+      <c r="U4" s="12">
+        <v>4</v>
+      </c>
+      <c r="V4" s="9">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="21">
+        <f t="shared" ref="Y4:Y16" si="3">X4</f>
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <f t="shared" ref="Z4:Z10" si="4">X4</f>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="12">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="21">
+        <v>6</v>
+      </c>
+      <c r="F5" s="21">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3">
+        <v>18</v>
+      </c>
+      <c r="H5" s="3">
+        <v>18</v>
+      </c>
+      <c r="T5" t="s">
+        <v>166</v>
+      </c>
+      <c r="U5" s="12">
+        <v>3</v>
+      </c>
+      <c r="V5" s="9">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="12">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9">
+        <f>SUM(D6:O6)</f>
+        <v>24</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="T6" t="s">
+        <v>108</v>
+      </c>
+      <c r="U6" s="12">
+        <v>2</v>
+      </c>
+      <c r="V6" s="9">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y6" s="21">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="Z6" s="3">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="AA6" s="3"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="D7" s="3">
+        <v>12</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7">
+        <v>20</v>
+      </c>
+      <c r="J7">
+        <v>60</v>
+      </c>
+      <c r="T7" t="s">
+        <v>168</v>
+      </c>
+      <c r="U7" s="12">
+        <v>1</v>
+      </c>
+      <c r="V7" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z7" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA7" s="3"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="12">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="21">
+        <v>10</v>
+      </c>
+      <c r="F8" s="21">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3">
+        <v>30</v>
+      </c>
+      <c r="H8" s="3">
+        <v>30</v>
+      </c>
+      <c r="I8" s="3">
+        <v>30</v>
+      </c>
+      <c r="T8" t="s">
+        <v>167</v>
+      </c>
+      <c r="U8" s="12">
+        <v>1</v>
+      </c>
+      <c r="V8" s="9">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="12">
+        <v>4</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="21">
+        <v>4</v>
+      </c>
+      <c r="F9" s="21">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="T9" t="s">
+        <v>113</v>
+      </c>
+      <c r="U9" s="12">
+        <v>4</v>
+      </c>
+      <c r="V9" s="9">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10">
+        <v>18</v>
+      </c>
+      <c r="F10">
+        <v>18</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="T10" t="s">
+        <v>171</v>
+      </c>
+      <c r="U10" s="12">
+        <v>1</v>
+      </c>
+      <c r="V10" s="9">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3">
+        <v>6</v>
+      </c>
+      <c r="Y10" s="21">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="Z10" s="3">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AA10" s="3"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="12">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="21">
+        <v>44</v>
+      </c>
+      <c r="F11" s="21">
+        <v>44</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="L11">
+        <v>24</v>
+      </c>
+      <c r="T11" t="s">
+        <v>149</v>
+      </c>
+      <c r="U11" s="12">
+        <v>1</v>
+      </c>
+      <c r="V11" s="9">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="W11" s="3">
+        <v>8</v>
+      </c>
+      <c r="X11" s="3">
+        <v>12</v>
+      </c>
+      <c r="Y11" s="21">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="Z11" s="3">
+        <f t="shared" ref="Z11:Z16" si="5">X11</f>
+        <v>12</v>
+      </c>
+      <c r="AA11" s="3"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="21">
+        <v>40</v>
+      </c>
+      <c r="F12" s="21">
+        <v>40</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="L12">
+        <v>24</v>
+      </c>
+      <c r="T12" t="s">
+        <v>172</v>
+      </c>
+      <c r="U12" s="12">
+        <v>1</v>
+      </c>
+      <c r="V12" s="9">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="W12" s="3">
+        <v>4</v>
+      </c>
+      <c r="X12" s="3">
+        <v>12</v>
+      </c>
+      <c r="Y12" s="21">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="Z12" s="3">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="AA12" s="3"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="C13" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="3"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="3"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B15" s="12"/>
+      <c r="C15" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="3"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B16" s="12"/>
+      <c r="C16" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L21" s="20"/>
+    </row>
+    <row r="22" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L22" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>